<commit_message>
modify the interface document
</commit_message>
<xml_diff>
--- a/接口文档.xlsx
+++ b/接口文档.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84589\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\yuelugame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20628880-A697-4DD4-9AC1-7B83DA3EE2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A8F3CB-7CAF-48DD-AFB3-760659FCD1C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,11 +71,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>account:"1001"
-password:"12345"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>{
     "code":0,
     "message":"请求成功",
@@ -98,12 +93,6 @@
   </si>
   <si>
     <t>注册一个新账户，系统返回用户账号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">username:"orchid"
-password:"123456"
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -157,6 +146,20 @@
   </si>
   <si>
     <t>/games/games_list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "account":"1001",
+    "password":"123456"
+}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    "name":"orchid",
+    "password":"123456"
+}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -225,10 +228,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,7 +516,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -521,7 +524,7 @@
     <col min="1" max="1" width="17.625" customWidth="1"/>
     <col min="2" max="2" width="15.25" customWidth="1"/>
     <col min="4" max="4" width="11.375" customWidth="1"/>
-    <col min="5" max="5" width="21.25" customWidth="1"/>
+    <col min="5" max="5" width="25.125" customWidth="1"/>
     <col min="6" max="6" width="41.625" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
@@ -551,7 +554,7 @@
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -564,55 +567,55 @@
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="149.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+      <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="G3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="211.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>